<commit_message>
new template for demo
</commit_message>
<xml_diff>
--- a/backend/sample/excel/Complex_Translated_Demo.xlsx
+++ b/backend/sample/excel/Complex_Translated_Demo.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Lee\Desktop\GS Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDFFCE5-12A8-4373-B05F-C4F58279C501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D97C825-18D0-402E-B055-629CA1A3A168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" tabRatio="603" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
     <sheet name="Stock Balance" sheetId="4" r:id="rId2"/>
     <sheet name="Demo tables beside" sheetId="6" r:id="rId3"/>
+    <sheet name="Simple" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="EQPosnDate">'Stock Balance'!#REF!</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
   <si>
     <t>Company Name</t>
     <phoneticPr fontId="3"/>
@@ -331,17 +332,148 @@
   </si>
   <si>
     <t>##totalTransDaysOutflow</t>
+  </si>
+  <si>
+    <t>positionDate</t>
+  </si>
+  <si>
+    <t>!!&gt; positionDate</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>!!&gt; portfolio</t>
+  </si>
+  <si>
+    <t>instrumentType</t>
+  </si>
+  <si>
+    <t>!!&gt; instrumentType</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>!!&gt; ISIN</t>
+  </si>
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>!!&gt; ticker</t>
+  </si>
+  <si>
+    <t>contractCode</t>
+  </si>
+  <si>
+    <t>!!&gt; contractCode --</t>
+  </si>
+  <si>
+    <t>coupon</t>
+  </si>
+  <si>
+    <t>!!&gt; coupon</t>
+  </si>
+  <si>
+    <t>maturity</t>
+  </si>
+  <si>
+    <t>!!&gt; maturityDate</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!&gt; currency </t>
+  </si>
+  <si>
+    <t>currentFace</t>
+  </si>
+  <si>
+    <t>!!&gt; currentFace</t>
+  </si>
+  <si>
+    <t>originalFace</t>
+  </si>
+  <si>
+    <t>!!&gt; originalFace</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>!!&gt; price</t>
+  </si>
+  <si>
+    <t>marketValue</t>
+  </si>
+  <si>
+    <t>!!&gt; marketValue</t>
+  </si>
+  <si>
+    <t>!!v positionDate</t>
+  </si>
+  <si>
+    <t>!!v portfolio</t>
+  </si>
+  <si>
+    <t>!!v instrumentType</t>
+  </si>
+  <si>
+    <t>!!v ISIN</t>
+  </si>
+  <si>
+    <t>!!v ticker</t>
+  </si>
+  <si>
+    <t>!!v coupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!v currency </t>
+  </si>
+  <si>
+    <t>!!v currentFace</t>
+  </si>
+  <si>
+    <t>!!v originalFace</t>
+  </si>
+  <si>
+    <t>!!v price</t>
+  </si>
+  <si>
+    <t>!!v marketValue</t>
+  </si>
+  <si>
+    <t>!!v contractCode ++</t>
+  </si>
+  <si>
+    <t>!!&gt; security_cd</t>
+  </si>
+  <si>
+    <t>!!&gt; securityDescription</t>
+  </si>
+  <si>
+    <t>!!&gt;</t>
+  </si>
+  <si>
+    <t>!!&gt; market_value_bs</t>
+  </si>
+  <si>
+    <t>!!&gt; trade_ccy_cd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0_ "/>
+    <numFmt numFmtId="166" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="167" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -603,8 +735,27 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -827,8 +978,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.24988555558946501"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="37">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1304,6 +1461,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1410,7 +1602,7 @@
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1660,6 +1852,126 @@
     </xf>
     <xf numFmtId="38" fontId="2" fillId="31" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="41" fillId="38" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="77" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="41" fillId="38" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="41" fillId="38" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="38" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="41" fillId="38" borderId="6" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="6" fillId="0" borderId="37" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="42" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="77" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="6" fillId="0" borderId="0" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="41" fillId="38" borderId="38" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="41" fillId="38" borderId="39" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="41" fillId="38" borderId="39" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="41" fillId="38" borderId="39" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="41" fillId="38" borderId="39" xfId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="39" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="43" fillId="0" borderId="0" xfId="30" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="6" fillId="0" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2307,7 +2619,7 @@
   </sheetPr>
   <dimension ref="B2:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -2331,17 +2643,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2355,10 +2667,10 @@
         <v>53</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="96" t="s">
+      <c r="G3" s="136" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="96"/>
+      <c r="H3" s="136"/>
       <c r="I3" s="5" t="s">
         <v>74</v>
       </c>
@@ -2376,10 +2688,10 @@
       <c r="F4" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="96" t="s">
+      <c r="G4" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="96"/>
+      <c r="H4" s="136"/>
       <c r="I4" s="37" t="s">
         <v>75</v>
       </c>
@@ -2398,10 +2710,10 @@
       <c r="F5" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="96" t="s">
+      <c r="G5" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="96"/>
+      <c r="H5" s="136"/>
       <c r="I5" s="37" t="s">
         <v>76</v>
       </c>
@@ -2410,35 +2722,35 @@
     </row>
     <row r="6" spans="2:15" ht="14.25" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="86"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="90" t="s">
+      <c r="B7" s="126"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="85" t="s">
+      <c r="E7" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85" t="s">
+      <c r="F7" s="125"/>
+      <c r="G7" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="85"/>
-      <c r="I7" s="92" t="s">
+      <c r="H7" s="125"/>
+      <c r="I7" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="94" t="s">
+      <c r="J7" s="134" t="s">
         <v>32</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="97" t="s">
+      <c r="L7" s="137" t="s">
         <v>43</v>
       </c>
       <c r="N7" s="66"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="88"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="91"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="131"/>
       <c r="E8" s="13" t="s">
         <v>29</v>
       </c>
@@ -2451,10 +2763,10 @@
       <c r="H8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="93"/>
-      <c r="J8" s="95"/>
+      <c r="I8" s="133"/>
+      <c r="J8" s="135"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="98"/>
+      <c r="L8" s="138"/>
     </row>
     <row r="9" spans="2:15" ht="67.5">
       <c r="B9" s="50" t="s">
@@ -2608,20 +2920,20 @@
       <c r="I18" s="36"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="99"/>
+      <c r="C20" s="139"/>
       <c r="I20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="69"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="100" t="s">
+      <c r="B21" s="140" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="101"/>
+      <c r="C21" s="141"/>
       <c r="D21" s="58" t="s">
         <v>58</v>
       </c>
@@ -2634,10 +2946,10 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="142" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="103"/>
+      <c r="C22" s="143"/>
       <c r="D22" s="54" t="s">
         <v>59</v>
       </c>
@@ -2650,10 +2962,10 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="102" t="s">
+      <c r="B23" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="103"/>
+      <c r="C23" s="143"/>
       <c r="D23" s="54" t="s">
         <v>57</v>
       </c>
@@ -2665,10 +2977,10 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="148" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="109"/>
+      <c r="C24" s="149"/>
       <c r="D24" s="61" t="s">
         <v>56</v>
       </c>
@@ -2682,28 +2994,28 @@
       <c r="K24" s="68"/>
     </row>
     <row r="27" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="139" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="99"/>
-      <c r="D27" s="99"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="99"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="139"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="139"/>
     </row>
     <row r="28" spans="2:11" ht="40.5">
-      <c r="B28" s="110"/>
-      <c r="C28" s="111"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="151"/>
       <c r="D28" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="92" t="s">
+      <c r="E28" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="92"/>
-      <c r="G28" s="92" t="s">
+      <c r="F28" s="132"/>
+      <c r="G28" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="104"/>
+      <c r="H28" s="144"/>
       <c r="I28" s="72" t="s">
         <v>22</v>
       </c>
@@ -2712,15 +3024,15 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B29" s="112" t="s">
+      <c r="B29" s="152" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="113"/>
+      <c r="C29" s="153"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="105"/>
+      <c r="E29" s="145"/>
+      <c r="F29" s="145"/>
+      <c r="G29" s="145"/>
+      <c r="H29" s="145"/>
       <c r="I29" s="18">
         <f>E29 - D29</f>
         <v>0</v>
@@ -2736,10 +3048,10 @@
       <c r="J30" s="68"/>
     </row>
     <row r="31" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B31" s="106" t="s">
+      <c r="B31" s="146" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="107"/>
+      <c r="C31" s="147"/>
       <c r="D31" s="22"/>
       <c r="G31" s="31"/>
     </row>
@@ -3034,14 +3346,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87636DA9-6C02-43F4-8ADF-4043CF9FB476}">
-  <dimension ref="B2:M26"/>
+  <dimension ref="B2:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
+    <col min="1" max="1" width="6.625" customWidth="1"/>
+    <col min="2" max="2" width="9.25" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="13.125" customWidth="1"/>
     <col min="13" max="13" width="19.25" customWidth="1"/>
@@ -3049,30 +3365,30 @@
   <sheetData>
     <row r="2" spans="2:13" ht="14.25" thickBot="1"/>
     <row r="3" spans="2:13">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="90" t="s">
+      <c r="B3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="125" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85" t="s">
+      <c r="F3" s="125"/>
+      <c r="G3" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="92" t="s">
+      <c r="H3" s="125"/>
+      <c r="I3" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="134" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="88"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="91"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="129"/>
+      <c r="D4" s="131"/>
       <c r="E4" s="13" t="s">
         <v>29</v>
       </c>
@@ -3085,8 +3401,8 @@
       <c r="H4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="93"/>
-      <c r="J4" s="95"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="135"/>
     </row>
     <row r="5" spans="2:13" ht="40.5">
       <c r="B5" s="50" t="s">
@@ -3370,6 +3686,78 @@
       <c r="H26" s="81"/>
       <c r="I26" s="81"/>
     </row>
+    <row r="28" spans="3:9">
+      <c r="C28" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+    </row>
+    <row r="29" spans="3:9" ht="40.5">
+      <c r="C29" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+    </row>
+    <row r="30" spans="3:9">
+      <c r="C30" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+    </row>
+    <row r="31" spans="3:9">
+      <c r="C31" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+    </row>
+    <row r="32" spans="3:9" ht="27">
+      <c r="C32" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+    </row>
+    <row r="33" spans="3:8">
+      <c r="C33" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="64" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="J3:J4"/>
@@ -3380,6 +3768,856 @@
     <mergeCell ref="I3:I4"/>
   </mergeCells>
   <phoneticPr fontId="40" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE7B166-A50F-4163-AA09-67AF12D7EFF6}">
+  <dimension ref="A1:S35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15">
+      <c r="A1" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="88"/>
+      <c r="O1" s="88"/>
+      <c r="P1" s="88"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+    </row>
+    <row r="2" spans="1:19" ht="15">
+      <c r="A2" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+    </row>
+    <row r="3" spans="1:19" ht="15">
+      <c r="A3" s="89" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="86" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="86"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="88"/>
+      <c r="R3" s="88"/>
+      <c r="S3" s="88"/>
+    </row>
+    <row r="4" spans="1:19" ht="15">
+      <c r="A4" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+    </row>
+    <row r="5" spans="1:19" ht="15">
+      <c r="A5" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="88"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
+    </row>
+    <row r="6" spans="1:19" ht="15">
+      <c r="A6" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="88"/>
+      <c r="S6" s="88"/>
+    </row>
+    <row r="7" spans="1:19" ht="15">
+      <c r="A7" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="86"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+    </row>
+    <row r="8" spans="1:19" ht="15">
+      <c r="A8" s="84" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="88"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="87"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="88"/>
+      <c r="O8" s="88"/>
+      <c r="P8" s="88"/>
+      <c r="Q8" s="88"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="88"/>
+    </row>
+    <row r="9" spans="1:19" ht="15">
+      <c r="A9" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="86"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
+      <c r="R9" s="88"/>
+      <c r="S9" s="88"/>
+    </row>
+    <row r="10" spans="1:19" ht="15">
+      <c r="A10" s="92" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="86"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="85"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="85"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85"/>
+      <c r="L10" s="85"/>
+      <c r="M10" s="85"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="88"/>
+      <c r="S10" s="88"/>
+    </row>
+    <row r="11" spans="1:19" ht="15">
+      <c r="A11" s="93" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="85"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
+      <c r="S11" s="88"/>
+    </row>
+    <row r="12" spans="1:19" ht="15">
+      <c r="A12" s="89" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="86"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="85"/>
+      <c r="M12" s="85"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="88"/>
+      <c r="S12" s="88"/>
+    </row>
+    <row r="13" spans="1:19" ht="15">
+      <c r="A13" s="89" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="86"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="88"/>
+      <c r="S13" s="88"/>
+    </row>
+    <row r="14" spans="1:19" ht="14.25">
+      <c r="A14" s="94"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="96"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+      <c r="S14" s="102"/>
+    </row>
+    <row r="15" spans="1:19" ht="14.25">
+      <c r="A15" s="103"/>
+      <c r="B15" s="104"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="106"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="108"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="106"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="110"/>
+      <c r="L15" s="110"/>
+      <c r="M15" s="110"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="102"/>
+      <c r="P15" s="102"/>
+      <c r="Q15" s="102"/>
+      <c r="R15" s="102"/>
+      <c r="S15" s="102"/>
+    </row>
+    <row r="16" spans="1:19" ht="14.25">
+      <c r="A16" s="103"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="108"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="110"/>
+      <c r="K16" s="110"/>
+      <c r="L16" s="110"/>
+      <c r="M16" s="110"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
+      <c r="P16" s="102"/>
+      <c r="Q16" s="102"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="102"/>
+    </row>
+    <row r="17" spans="1:19" ht="15">
+      <c r="A17" s="111" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="112" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="112" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="112" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="112" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="113" t="s">
+        <v>103</v>
+      </c>
+      <c r="G17" s="112" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="114" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="115" t="s">
+        <v>111</v>
+      </c>
+      <c r="J17" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="K17" s="112" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="102"/>
+    </row>
+    <row r="18" spans="1:19" ht="14.25">
+      <c r="A18" s="116" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="117" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="118" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="117" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="119" t="s">
+        <v>122</v>
+      </c>
+      <c r="G18" s="118" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="120" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="120" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="120" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" s="120" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="121" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="102"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="102"/>
+      <c r="P18" s="102"/>
+      <c r="Q18" s="102"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="102"/>
+    </row>
+    <row r="19" spans="1:19" ht="14.25">
+      <c r="A19" s="116"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="119"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="120"/>
+      <c r="I19" s="120"/>
+      <c r="J19" s="120"/>
+      <c r="K19" s="120"/>
+      <c r="L19" s="121"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="102"/>
+      <c r="O19" s="102"/>
+      <c r="P19" s="102"/>
+      <c r="Q19" s="102"/>
+      <c r="R19" s="102"/>
+      <c r="S19" s="102"/>
+    </row>
+    <row r="20" spans="1:19" ht="14.25">
+      <c r="A20" s="116"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="118"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="119"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="120"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="120"/>
+      <c r="K20" s="120"/>
+      <c r="L20" s="121"/>
+      <c r="M20" s="122"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="102"/>
+      <c r="P20" s="102"/>
+      <c r="Q20" s="102"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="102"/>
+    </row>
+    <row r="21" spans="1:19" ht="14.25">
+      <c r="A21" s="116"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="117"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="118"/>
+      <c r="H21" s="120"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="120"/>
+      <c r="K21" s="120"/>
+      <c r="L21" s="121"/>
+      <c r="M21" s="122"/>
+      <c r="N21" s="102"/>
+      <c r="O21" s="102"/>
+      <c r="P21" s="102"/>
+      <c r="Q21" s="102"/>
+      <c r="R21" s="102"/>
+      <c r="S21" s="102"/>
+    </row>
+    <row r="22" spans="1:19" ht="14.25">
+      <c r="A22" s="116"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
+      <c r="E22" s="117"/>
+      <c r="F22" s="119"/>
+      <c r="G22" s="118"/>
+      <c r="H22" s="120"/>
+      <c r="I22" s="120"/>
+      <c r="J22" s="120"/>
+      <c r="K22" s="120"/>
+      <c r="L22" s="121"/>
+      <c r="M22" s="122"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="102"/>
+      <c r="P22" s="102"/>
+      <c r="Q22" s="102"/>
+      <c r="R22" s="102"/>
+      <c r="S22" s="102"/>
+    </row>
+    <row r="23" spans="1:19" ht="14.25">
+      <c r="A23" s="116"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="118"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="120"/>
+      <c r="I23" s="120"/>
+      <c r="J23" s="120"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="121"/>
+      <c r="M23" s="122"/>
+      <c r="N23" s="102"/>
+      <c r="O23" s="102"/>
+      <c r="P23" s="102"/>
+      <c r="Q23" s="102"/>
+      <c r="R23" s="102"/>
+      <c r="S23" s="102"/>
+    </row>
+    <row r="24" spans="1:19" ht="14.25">
+      <c r="A24" s="116"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="117"/>
+      <c r="D24" s="118"/>
+      <c r="E24" s="117"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="118"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="121"/>
+      <c r="M24" s="122"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="102"/>
+      <c r="Q24" s="102"/>
+      <c r="R24" s="102"/>
+      <c r="S24" s="102"/>
+    </row>
+    <row r="25" spans="1:19" ht="14.25">
+      <c r="A25" s="116"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="117"/>
+      <c r="D25" s="118"/>
+      <c r="E25" s="117"/>
+      <c r="F25" s="119"/>
+      <c r="G25" s="118"/>
+      <c r="H25" s="120"/>
+      <c r="I25" s="120"/>
+      <c r="J25" s="120"/>
+      <c r="K25" s="120"/>
+      <c r="L25" s="123"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="102"/>
+      <c r="P25" s="102"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="102"/>
+      <c r="S25" s="102"/>
+    </row>
+    <row r="26" spans="1:19" ht="14.25">
+      <c r="A26" s="116"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="118"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="119"/>
+      <c r="G26" s="118"/>
+      <c r="H26" s="120"/>
+      <c r="I26" s="120"/>
+      <c r="J26" s="120"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="123"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="102"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="102"/>
+      <c r="Q26" s="102"/>
+      <c r="R26" s="102"/>
+      <c r="S26" s="102"/>
+    </row>
+    <row r="27" spans="1:19" ht="14.25">
+      <c r="A27" s="116"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="119"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="123"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="102"/>
+      <c r="O27" s="102"/>
+      <c r="P27" s="102"/>
+      <c r="Q27" s="102"/>
+      <c r="R27" s="102"/>
+      <c r="S27" s="102"/>
+    </row>
+    <row r="28" spans="1:19" ht="14.25">
+      <c r="A28" s="116"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="119"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="120"/>
+      <c r="I28" s="120"/>
+      <c r="J28" s="120"/>
+      <c r="K28" s="120"/>
+      <c r="L28" s="123"/>
+      <c r="M28" s="122"/>
+      <c r="N28" s="102"/>
+      <c r="O28" s="102"/>
+      <c r="P28" s="102"/>
+      <c r="Q28" s="102"/>
+      <c r="R28" s="102"/>
+      <c r="S28" s="102"/>
+    </row>
+    <row r="29" spans="1:19" ht="14.25">
+      <c r="A29" s="116"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="119"/>
+      <c r="G29" s="118"/>
+      <c r="H29" s="120"/>
+      <c r="I29" s="120"/>
+      <c r="J29" s="120"/>
+      <c r="K29" s="120"/>
+      <c r="L29" s="123"/>
+      <c r="M29" s="122"/>
+      <c r="N29" s="102"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="102"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="102"/>
+    </row>
+    <row r="30" spans="1:19" ht="14.25">
+      <c r="A30" s="116"/>
+      <c r="B30" s="86"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="118"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="120"/>
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="123"/>
+      <c r="M30" s="122"/>
+      <c r="N30" s="102"/>
+      <c r="O30" s="102"/>
+      <c r="P30" s="102"/>
+      <c r="Q30" s="102"/>
+      <c r="R30" s="102"/>
+      <c r="S30" s="102"/>
+    </row>
+    <row r="31" spans="1:19" ht="14.25">
+      <c r="A31" s="116"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="117"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="117"/>
+      <c r="F31" s="119"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="120"/>
+      <c r="I31" s="120"/>
+      <c r="J31" s="120"/>
+      <c r="K31" s="120"/>
+      <c r="L31" s="123"/>
+      <c r="M31" s="122"/>
+      <c r="N31" s="102"/>
+      <c r="O31" s="102"/>
+      <c r="P31" s="102"/>
+      <c r="Q31" s="102"/>
+      <c r="R31" s="102"/>
+      <c r="S31" s="102"/>
+    </row>
+    <row r="32" spans="1:19" ht="14.25">
+      <c r="A32" s="116"/>
+      <c r="B32" s="86"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="118"/>
+      <c r="E32" s="117"/>
+      <c r="F32" s="119"/>
+      <c r="G32" s="118"/>
+      <c r="H32" s="120"/>
+      <c r="I32" s="120"/>
+      <c r="J32" s="120"/>
+      <c r="K32" s="120"/>
+      <c r="L32" s="123"/>
+      <c r="M32" s="122"/>
+      <c r="N32" s="102"/>
+      <c r="O32" s="102"/>
+      <c r="P32" s="102"/>
+      <c r="Q32" s="102"/>
+      <c r="R32" s="102"/>
+      <c r="S32" s="102"/>
+    </row>
+    <row r="33" spans="1:19" ht="14.25">
+      <c r="A33" s="116"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="117"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="119"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="120"/>
+      <c r="I33" s="120"/>
+      <c r="J33" s="120"/>
+      <c r="K33" s="120"/>
+      <c r="L33" s="123"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="102"/>
+      <c r="O33" s="102"/>
+      <c r="P33" s="102"/>
+      <c r="Q33" s="102"/>
+      <c r="R33" s="102"/>
+      <c r="S33" s="102"/>
+    </row>
+    <row r="34" spans="1:19" ht="14.25">
+      <c r="A34" s="116"/>
+      <c r="B34" s="86"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="120"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="120"/>
+      <c r="K34" s="120"/>
+      <c r="L34" s="123"/>
+      <c r="M34" s="122"/>
+      <c r="N34" s="102"/>
+      <c r="O34" s="102"/>
+      <c r="P34" s="102"/>
+      <c r="Q34" s="102"/>
+      <c r="R34" s="102"/>
+      <c r="S34" s="102"/>
+    </row>
+    <row r="35" spans="1:19" ht="14.25">
+      <c r="A35" s="116"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="118"/>
+      <c r="E35" s="117"/>
+      <c r="F35" s="119"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="120"/>
+      <c r="I35" s="120"/>
+      <c r="J35" s="120"/>
+      <c r="K35" s="120"/>
+      <c r="L35" s="123"/>
+      <c r="M35" s="122"/>
+      <c r="N35" s="102"/>
+      <c r="O35" s="102"/>
+      <c r="P35" s="102"/>
+      <c r="Q35" s="102"/>
+      <c r="R35" s="102"/>
+      <c r="S35" s="102"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add load testing suite
</commit_message>
<xml_diff>
--- a/backend/sample/excel/Complex_Translated_Demo.xlsx
+++ b/backend/sample/excel/Complex_Translated_Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Lee\Desktop\GS Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Documents\GitHub\repositories\Rendr\backend\sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D97C825-18D0-402E-B055-629CA1A3A168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAE78C0-CAF4-4926-B4D4-6747847156C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="2250" windowWidth="19455" windowHeight="12780" tabRatio="603" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pension Investment Status" sheetId="3" r:id="rId1"/>
@@ -1973,6 +1973,60 @@
     <xf numFmtId="40" fontId="6" fillId="0" borderId="6" xfId="30" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1997,9 +2051,6 @@
     <xf numFmtId="38" fontId="2" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="38" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2011,57 +2062,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="2" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="88">
@@ -2643,17 +2643,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="27" customHeight="1">
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="142" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="124"/>
-      <c r="G2" s="124"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="124"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:15" ht="13.5" customHeight="1" thickBot="1">
@@ -2667,10 +2667,10 @@
         <v>53</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="136" t="s">
+      <c r="G3" s="153" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="136"/>
+      <c r="H3" s="153"/>
       <c r="I3" s="5" t="s">
         <v>74</v>
       </c>
@@ -2688,10 +2688,10 @@
       <c r="F4" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="136" t="s">
+      <c r="G4" s="153" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="136"/>
+      <c r="H4" s="153"/>
       <c r="I4" s="37" t="s">
         <v>75</v>
       </c>
@@ -2710,10 +2710,10 @@
       <c r="F5" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="136" t="s">
+      <c r="G5" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="136"/>
+      <c r="H5" s="153"/>
       <c r="I5" s="37" t="s">
         <v>76</v>
       </c>
@@ -2722,35 +2722,35 @@
     </row>
     <row r="6" spans="2:15" ht="14.25" thickBot="1"/>
     <row r="7" spans="2:15" ht="13.5" customHeight="1">
-      <c r="B7" s="126"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="130" t="s">
+      <c r="B7" s="144"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="125" t="s">
+      <c r="E7" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125" t="s">
+      <c r="F7" s="143"/>
+      <c r="G7" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="125"/>
-      <c r="I7" s="132" t="s">
+      <c r="H7" s="143"/>
+      <c r="I7" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="134" t="s">
+      <c r="J7" s="151" t="s">
         <v>32</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="137" t="s">
+      <c r="L7" s="136" t="s">
         <v>43</v>
       </c>
       <c r="N7" s="66"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="128"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="131"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="13" t="s">
         <v>29</v>
       </c>
@@ -2763,10 +2763,10 @@
       <c r="H8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="133"/>
-      <c r="J8" s="135"/>
+      <c r="I8" s="150"/>
+      <c r="J8" s="152"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="138"/>
+      <c r="L8" s="137"/>
     </row>
     <row r="9" spans="2:15" ht="67.5">
       <c r="B9" s="50" t="s">
@@ -2920,20 +2920,20 @@
       <c r="I18" s="36"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1" thickBot="1">
-      <c r="B20" s="139" t="s">
+      <c r="B20" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="139"/>
+      <c r="C20" s="135"/>
       <c r="I20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="69"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="140" t="s">
+      <c r="B21" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="141"/>
+      <c r="C21" s="139"/>
       <c r="D21" s="58" t="s">
         <v>58</v>
       </c>
@@ -2946,10 +2946,10 @@
       </c>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="143"/>
+      <c r="C22" s="141"/>
       <c r="D22" s="54" t="s">
         <v>59</v>
       </c>
@@ -2962,10 +2962,10 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="142" t="s">
+      <c r="B23" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="143"/>
+      <c r="C23" s="141"/>
       <c r="D23" s="54" t="s">
         <v>57</v>
       </c>
@@ -2977,10 +2977,10 @@
       </c>
     </row>
     <row r="24" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B24" s="148" t="s">
+      <c r="B24" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="149"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="61" t="s">
         <v>56</v>
       </c>
@@ -2994,28 +2994,28 @@
       <c r="K24" s="68"/>
     </row>
     <row r="27" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B27" s="139" t="s">
+      <c r="B27" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="139"/>
-      <c r="D27" s="139"/>
-      <c r="E27" s="139"/>
-      <c r="F27" s="139"/>
+      <c r="C27" s="135"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
+      <c r="F27" s="135"/>
     </row>
     <row r="28" spans="2:11" ht="40.5">
-      <c r="B28" s="150"/>
-      <c r="C28" s="151"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="132"/>
       <c r="D28" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="132" t="s">
+      <c r="E28" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="132"/>
-      <c r="G28" s="132" t="s">
+      <c r="F28" s="124"/>
+      <c r="G28" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="144"/>
+      <c r="H28" s="125"/>
       <c r="I28" s="72" t="s">
         <v>22</v>
       </c>
@@ -3024,15 +3024,15 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B29" s="152" t="s">
+      <c r="B29" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="153"/>
+      <c r="C29" s="134"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="145"/>
-      <c r="F29" s="145"/>
-      <c r="G29" s="145"/>
-      <c r="H29" s="145"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="126"/>
       <c r="I29" s="18">
         <f>E29 - D29</f>
         <v>0</v>
@@ -3048,10 +3048,10 @@
       <c r="J30" s="68"/>
     </row>
     <row r="31" spans="2:11" ht="14.25" thickBot="1">
-      <c r="B31" s="146" t="s">
+      <c r="B31" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="147"/>
+      <c r="C31" s="128"/>
       <c r="D31" s="22"/>
       <c r="G31" s="31"/>
     </row>
@@ -3081,20 +3081,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
@@ -3105,6 +3091,20 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <printOptions horizontalCentered="1"/>
@@ -3349,7 +3349,7 @@
   <dimension ref="B2:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3365,30 +3365,30 @@
   <sheetData>
     <row r="2" spans="2:13" ht="14.25" thickBot="1"/>
     <row r="3" spans="2:13">
-      <c r="B3" s="126"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="130" t="s">
+      <c r="B3" s="144"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="125" t="s">
+      <c r="E3" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125" t="s">
+      <c r="F3" s="143"/>
+      <c r="G3" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="125"/>
-      <c r="I3" s="132" t="s">
+      <c r="H3" s="143"/>
+      <c r="I3" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="134" t="s">
+      <c r="J3" s="151" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="128"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="131"/>
+      <c r="B4" s="146"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="149"/>
       <c r="E4" s="13" t="s">
         <v>29</v>
       </c>
@@ -3401,8 +3401,8 @@
       <c r="H4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="133"/>
-      <c r="J4" s="135"/>
+      <c r="I4" s="150"/>
+      <c r="J4" s="152"/>
     </row>
     <row r="5" spans="2:13" ht="40.5">
       <c r="B5" s="50" t="s">
@@ -3526,10 +3526,7 @@
         <f>SUM(D5:D11)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="25">
-        <f>+D17</f>
-        <v>0</v>
-      </c>
+      <c r="E12" s="25"/>
       <c r="F12" s="56"/>
       <c r="G12" s="25"/>
       <c r="H12" s="56"/>
@@ -4623,21 +4620,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CDC787A71DDF645B3B1EC4B4C087709" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfcc5dabae62faba7569d214b4f3e22c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -4751,17 +4733,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4775,17 +4773,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{835BF43D-5F5B-4A92-8B6A-74ACA0EB3617}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31452BF2-B3C4-4EBE-BE76-B62708FA3B9D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>